<commit_message>
one pager and new positioning
</commit_message>
<xml_diff>
--- a/TRACKER.xlsx
+++ b/TRACKER.xlsx
@@ -4579,7 +4579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -5600,6 +5600,73 @@
       <c r="M15" s="20" t="inlineStr">
         <is>
           <t>Alto filtro.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Job Application</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Grey Matter Recruitment (Mobile AdTech Ecosystem)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>COO</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>🟡 Da applicare (Easy Apply)</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>75%</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Highly competitive + bonus + share options (stimato €120-180K+)</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Ops leadership high-growth B2B tech; delivery systems &amp; governance; cross-functional operating systems; data-literate; product-led thinking; reduce founder dependency</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>No AdTech/mobile advertising experience; product-led thinking (ops/finance-led, non product-led)</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Easy Apply su LinkedIn</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>68 applicanti in 1 settimana. Recruiter: Joe Hutton (SaaS &amp; AdTech specialist). DSP/SSP/Mediation/Game Publisher. 200% revenue growth 2023, targeting X10. VC-backed.</t>
         </is>
       </c>
     </row>

</xml_diff>